<commit_message>
Added waitbar to Generate button
</commit_message>
<xml_diff>
--- a/UserExports/info.xlsx
+++ b/UserExports/info.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4410" uniqueCount="4410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4452" uniqueCount="4452">
   <si>
     <t>Row</t>
   </si>
@@ -13216,6 +13216,132 @@
   </si>
   <si>
     <t>Scaffold Diameter (mm)</t>
+  </si>
+  <si>
+    <t>Pore Length: p (µm)</t>
+  </si>
+  <si>
+    <t>Pore Width: q (µm)</t>
+  </si>
+  <si>
+    <t>Pore Area: K (mm²)</t>
+  </si>
+  <si>
+    <t>Pore Perimeter: P (mm)</t>
+  </si>
+  <si>
+    <t>Major Pore Angle: A (deg)</t>
+  </si>
+  <si>
+    <t>Minor Pore Angle: B (deg)</t>
+  </si>
+  <si>
+    <t>Repeating Cells (X)</t>
+  </si>
+  <si>
+    <t>Repeating Cells (Y)</t>
+  </si>
+  <si>
+    <t>Original Geometry</t>
+  </si>
+  <si>
+    <t>Scaled Geometry</t>
+  </si>
+  <si>
+    <t>Fitted Geometry</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Scaffold Length (mm)</t>
+  </si>
+  <si>
+    <t>Scaffold Width (mm)</t>
+  </si>
+  <si>
+    <t>Pore Length: p (µm)</t>
+  </si>
+  <si>
+    <t>Pore Width: q (µm)</t>
+  </si>
+  <si>
+    <t>Pore Area: K (mm²)</t>
+  </si>
+  <si>
+    <t>Pore Perimeter: P (mm)</t>
+  </si>
+  <si>
+    <t>Major Pore Angle: A (deg)</t>
+  </si>
+  <si>
+    <t>Minor Pore Angle: B (deg)</t>
+  </si>
+  <si>
+    <t>Repeating Cells (X)</t>
+  </si>
+  <si>
+    <t>Repeating Cells (Y)</t>
+  </si>
+  <si>
+    <t>Original Geometry</t>
+  </si>
+  <si>
+    <t>Scaled Geometry</t>
+  </si>
+  <si>
+    <t>Fitted Geometry</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Scaffold Length (mm)</t>
+  </si>
+  <si>
+    <t>Scaffold Width (mm)</t>
+  </si>
+  <si>
+    <t>Pore Length: p (µm)</t>
+  </si>
+  <si>
+    <t>Pore Width: q (µm)</t>
+  </si>
+  <si>
+    <t>Pore Area: K (mm²)</t>
+  </si>
+  <si>
+    <t>Pore Perimeter: P (mm)</t>
+  </si>
+  <si>
+    <t>Major Pore Angle: A (deg)</t>
+  </si>
+  <si>
+    <t>Minor Pore Angle: B (deg)</t>
+  </si>
+  <si>
+    <t>Repeating Cells (X)</t>
+  </si>
+  <si>
+    <t>Repeating Cells (Y)</t>
+  </si>
+  <si>
+    <t>Original Geometry</t>
+  </si>
+  <si>
+    <t>Scaled Geometry</t>
+  </si>
+  <si>
+    <t>Fitted Geometry</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Scaffold Length (mm)</t>
+  </si>
+  <si>
+    <t>Scaffold Width (mm)</t>
   </si>
   <si>
     <t>Pore Length: p (µm)</t>
@@ -13574,127 +13700,121 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" customWidth="true"/>
-    <col min="2" max="2" width="15.93359375" customWidth="true"/>
-    <col min="3" max="3" width="14.93359375" customWidth="true"/>
-    <col min="4" max="4" width="14.37890625" customWidth="true"/>
+    <col min="1" max="1" width="22.44140625" customWidth="true"/>
+    <col min="2" max="2" width="16.34765625" customWidth="true"/>
+    <col min="3" max="3" width="15.16796875" customWidth="true"/>
+    <col min="4" max="4" width="14.62109375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>4396</v>
+        <v>4438</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>4407</v>
+        <v>4449</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>4408</v>
+        <v>4450</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>4409</v>
+        <v>4451</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>4397</v>
+        <v>4439</v>
       </c>
       <c r="B2" s="0">
-        <v>6</v>
+        <v>1000</v>
       </c>
       <c r="C2" s="0">
-        <v>6.9450000000000003</v>
+        <v>1000</v>
       </c>
       <c r="D2" s="0">
-        <v>6</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>4398</v>
+        <v>4440</v>
       </c>
       <c r="B3" s="0">
-        <v>6</v>
+        <v>1000</v>
       </c>
       <c r="C3" s="0">
-        <v>6</v>
+        <v>1000</v>
       </c>
       <c r="D3" s="0">
-        <v>6</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>4399</v>
+        <v>4441</v>
       </c>
       <c r="B4" s="0">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="C4" s="0">
-        <v>496.04199999999997</v>
+        <v>1000</v>
       </c>
       <c r="D4" s="0">
-        <v>500</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>4400</v>
+        <v>4442</v>
       </c>
       <c r="B5" s="0">
         <v>1000</v>
       </c>
       <c r="C5" s="0">
-        <v>992.08399999999995</v>
+        <v>1000</v>
       </c>
       <c r="D5" s="0">
-        <v>992.08399999999995</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>4401</v>
+        <v>4443</v>
       </c>
       <c r="B6" s="0">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C6" s="0">
-        <v>0.49199999999999999</v>
+        <v>1</v>
       </c>
       <c r="D6" s="0">
-        <v>0.496</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>4402</v>
+        <v>4444</v>
       </c>
       <c r="B7" s="0">
-        <v>3.8279999999999998</v>
+        <v>4</v>
       </c>
       <c r="C7" s="0">
-        <v>3.798</v>
+        <v>4</v>
       </c>
       <c r="D7" s="0">
-        <v>3.8170000000000002</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>4403</v>
+        <v>4445</v>
       </c>
-      <c r="B8" s="0">
-        <v>90</v>
-      </c>
-      <c r="C8" s="0">
-        <v>90</v>
-      </c>
-      <c r="D8" s="0">
-        <v>89.545000000000002</v>
-      </c>
+      <c r="B8" s="0"/>
+      <c r="C8" s="0"/>
+      <c r="D8" s="0"/>
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>4404</v>
+        <v>4446</v>
       </c>
       <c r="B9" s="0"/>
       <c r="C9" s="0"/>
@@ -13702,30 +13822,30 @@
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>4405</v>
+        <v>4447</v>
       </c>
       <c r="B10" s="0">
-        <v>6</v>
+        <v>500</v>
       </c>
       <c r="C10" s="0">
-        <v>7</v>
+        <v>500</v>
       </c>
       <c r="D10" s="0">
-        <v>6</v>
+        <v>500</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>4406</v>
+        <v>4448</v>
       </c>
       <c r="B11" s="0">
-        <v>19</v>
+        <v>500</v>
       </c>
       <c r="C11" s="0">
-        <v>19</v>
+        <v>500</v>
       </c>
       <c r="D11" s="0">
-        <v>19</v>
+        <v>500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>